<commit_message>
eddy ni 1977-1978 (update)
</commit_message>
<xml_diff>
--- a/_data/ni/ni7778/individueel_eindstand_dworp_12_7778.xlsx
+++ b/_data/ni/ni7778/individueel_eindstand_dworp_12_7778.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14340" windowHeight="10095" activeTab="9"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14340" windowHeight="10095"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="16" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="146">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -451,12 +451,6 @@
     <t>matchpunten: w 1 - g 0,5 - v 0</t>
   </si>
   <si>
-    <t>14?</t>
-  </si>
-  <si>
-    <t>20?</t>
-  </si>
-  <si>
     <t>501 CRE Charleroi 3</t>
   </si>
   <si>
@@ -467,6 +461,9 @@
   </si>
   <si>
     <t>(forfait)</t>
+  </si>
+  <si>
+    <t>21?</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1732,7 +1729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3674,9 +3671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD280"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3796,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>37</v>
@@ -4372,7 +4367,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C7" s="34">
         <v>4</v>
@@ -5332,7 +5327,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12" s="34">
         <v>6</v>
@@ -5376,9 +5371,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="R12" s="87" t="s">
-        <v>141</v>
-      </c>
+      <c r="R12" s="87"/>
       <c r="S12" s="47">
         <f>IF(C12="","",IF(C12&gt;$K4,1,IF(C12=$K4,0.5,0)))</f>
         <v>0</v>
@@ -6371,15 +6364,14 @@
         <v>78</v>
       </c>
       <c r="P19" s="71">
-        <f>IF(Info!B$10=0,0,SUM(S19:AD19))+IF(Info!B$11=0,0,2*SUM(S19:AD19))+IF(Info!B$12=0,0,SUM(AS19:BD19))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q19" s="36">
         <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="R19" s="87" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="S19" s="47">
         <f>IF(C19="","",IF(C19&gt;D18,1,IF(C19=D18,0.5,0)))</f>
@@ -15923,7 +15915,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -16655,7 +16647,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -17020,7 +17012,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -17367,7 +17359,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -19047,11 +19039,15 @@
         <v>94</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
       <c r="F15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="10">
+        <v>3</v>
+      </c>
       <c r="H15" s="19">
         <v>19372</v>
       </c>
@@ -19071,11 +19067,15 @@
         <v>95</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="10">
+        <v>2</v>
+      </c>
       <c r="F16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="10">
+        <v>2</v>
+      </c>
       <c r="H16" s="19" t="s">
         <v>52</v>
       </c>
@@ -19095,11 +19095,15 @@
         <v>96</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10">
+        <v>2</v>
+      </c>
       <c r="F17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="10">
+        <v>2</v>
+      </c>
       <c r="H17" s="19" t="s">
         <v>52</v>
       </c>
@@ -19119,11 +19123,15 @@
         <v>97</v>
       </c>
       <c r="D18" s="18"/>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12">
+        <v>3</v>
+      </c>
       <c r="F18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
       <c r="H18" s="19">
         <v>76325</v>
       </c>
@@ -19142,11 +19150,15 @@
         <v/>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="13">
+        <v>8</v>
+      </c>
       <c r="F19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="13">
+        <v>8</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="16">
         <f>IFERROR(AVERAGE(J15:J18),"")</f>

</xml_diff>